<commit_message>
Seguro Patrimonial (mudança #11)
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>Caso</t>
   </si>
@@ -173,13 +173,45 @@
   </si>
   <si>
     <t>Separar o Lucro Cessante para cada tipo de interdição e estimar diretamente o lucro cessante total por evento.</t>
+  </si>
+  <si>
+    <t>Mudança Necessária no Template de Dados</t>
+  </si>
+  <si>
+    <t>Estas Variáveis devem ser estimadas como parâmetros: LucroCessanteAcidenteObito
+LucroCessanteAcidenteOutros
+LucroCessanteInterdicaoFiscalizacao</t>
+  </si>
+  <si>
+    <t>GanhoQualidade deve ser estimados como parâmetros. Outras variáveis relacionadas podem ser estimadas (margem, produção projetada, variação em vendas).</t>
+  </si>
+  <si>
+    <t>GanhoProdutividade deve ser estimados como parâmetro.</t>
+  </si>
+  <si>
+    <t>Funcionários Desligados Iniciais não precisam ser coletados.</t>
+  </si>
+  <si>
+    <t>Nenhuma.</t>
+  </si>
+  <si>
+    <t>Coluna SEEDFixa deve estar presente na aba de parâmetros. Lista dos parâmetros sem SeedFIXA deve ser inserida em uma aba.</t>
+  </si>
+  <si>
+    <t>Backlog Pós-Piloto.</t>
+  </si>
+  <si>
+    <t>Aba de Parâmetros deve usar a distribuição "normaltruncada", e usar os parâmetros 3 e 4 como mínimo e máximo.</t>
+  </si>
+  <si>
+    <t>Informar variável DespesasSeguroPatrimonial como parâmetro.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +221,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -216,13 +263,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -539,321 +596,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="14.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="63.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="14.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="G2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="G3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="G4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="G5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="G6" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="3" t="s">
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>23</v>
+      <c r="G15" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Poisson para evento Raros
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>Caso</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Ganho de qualidade será estimado diretamente.</t>
   </si>
   <si>
-    <t>Mudança Implementada</t>
-  </si>
-  <si>
     <t>Produtividade</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
   </si>
   <si>
     <t>Implementar Regressões como etapa de pré-processamento.</t>
-  </si>
-  <si>
-    <t>Implementar distribuição de Poisson para os eventos.</t>
   </si>
   <si>
     <t>Regressão do FAP permite que percentis assumam valores maiores do que 100.</t>
@@ -205,22 +199,32 @@
   </si>
   <si>
     <t>Informar variável DespesasSeguroPatrimonial como parâmetro.</t>
+  </si>
+  <si>
+    <t>Implementar distribuição de Poisson para os eventos raros (onde não há histórico).</t>
+  </si>
+  <si>
+    <t>A variável "FuncionariosBase" deve ser incluida na aba "Configs", e é usada pelo modelo para normalizar a taxa de acidentes. O valor deve corresponder à média do número de funcionários projetados.</t>
+  </si>
+  <si>
+    <t>BRS</t>
+  </si>
+  <si>
+    <t>Arquivo do dado de entrada não contém as variáveis Desligamentos Voluntários.</t>
+  </si>
+  <si>
+    <t>Inserir a variável no arquivo de dados de entrada.</t>
+  </si>
+  <si>
+    <t>Mudança Implementada, Testar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -263,8 +267,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -272,14 +277,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -596,353 +594,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="14.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="63.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="5.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taxas de Gravidade e Frequencia - Inputs agora estão corretos.
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>Caso</t>
   </si>
@@ -147,17 +147,6 @@
   </si>
   <si>
     <t>Índices Máximos para Ganho de Receita por Imagem: Atualmente o índice máximo considerado é o ampliado. No entanto, o índice ampliado é de difícil sensibilidade para o usuário. Além disso, pode ser mais coerente retirar este limite, visto que o ganho será arbitrado.</t>
-  </si>
-  <si>
-    <t>Decidir</t>
-  </si>
-  <si>
-    <t>Decisão a tomar:
-1 - Utilizar os índices do FAP como parâmetro;
-2 - Não utilizar nenhum índice (sempre atribuir o Ganho arbitrado).</t>
-  </si>
-  <si>
-    <t>Imagem</t>
   </si>
   <si>
     <t>Interdição Operacional</t>
@@ -177,12 +166,6 @@
 LucroCessanteInterdicaoFiscalizacao</t>
   </si>
   <si>
-    <t>GanhoQualidade deve ser estimados como parâmetros. Outras variáveis relacionadas podem ser estimadas (margem, produção projetada, variação em vendas).</t>
-  </si>
-  <si>
-    <t>GanhoProdutividade deve ser estimados como parâmetro.</t>
-  </si>
-  <si>
     <t>Funcionários Desligados Iniciais não precisam ser coletados.</t>
   </si>
   <si>
@@ -217,6 +200,24 @@
   </si>
   <si>
     <t>Mudança Implementada, Testar</t>
+  </si>
+  <si>
+    <t>GanhoQualidade deve ser estimados como parâmetros. Outras variáveis relacionadas podem ser eliminadas (margem, produção projetada, variação em vendas).</t>
+  </si>
+  <si>
+    <t>GanhoProdutividade deve ser estimado como parâmetro.</t>
+  </si>
+  <si>
+    <t>Imagem, Índices de Frequência</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Usar padrão da NBR 14280: Taxa de Frequência e Gravidade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserir estas variáveis no template: TempoComputadoMedio (Parâmetro)
+DiasUteis (Dados Projetados)
+</t>
   </si>
 </sst>
 </file>
@@ -596,9 +597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +634,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -653,10 +654,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -676,10 +677,10 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -699,10 +700,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -722,10 +723,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -745,10 +746,10 @@
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -765,13 +766,13 @@
         <v>21</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -791,7 +792,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -811,10 +812,10 @@
         <v>26</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -834,10 +835,10 @@
         <v>28</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -857,7 +858,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -877,10 +878,10 @@
         <v>32</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -911,16 +912,19 @@
         <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>40</v>
+        <v>56</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -931,19 +935,19 @@
         <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -951,16 +955,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Definição para a Alteração dos Bs
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Caso</t>
   </si>
@@ -218,6 +218,12 @@
     <t xml:space="preserve">Inserir estas variáveis no template: TempoComputadoMedio (Parâmetro)
 DiasUteis (Dados Projetados)
 </t>
+  </si>
+  <si>
+    <t>O número de benefícios estimados de acordo com os eventos e de acordo com a tabela dos eventos não é aderente aos dados observados no FAP.</t>
+  </si>
+  <si>
+    <t>Calcular um Fator para cada benefício (B91, B92, B94) e os eventos típicos e doenças ocupacionais com afastamento maior do que 15 dias. Usar este fator para considerar que a geração de benefícios seguirá a mesma proporção no futuro.</t>
   </si>
 </sst>
 </file>
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -279,6 +285,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -595,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,6 +980,26 @@
         <v>22</v>
       </c>
     </row>
+    <row r="17" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{6E59EE85-8273-468A-A589-1946F5BAD21C}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Alterações nos Dados Iniciais
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
   <si>
     <t>Caso</t>
   </si>
@@ -224,6 +224,13 @@
   </si>
   <si>
     <t>Calcular um Fator para cada benefício (B91, B92, B94) e os eventos típicos e doenças ocupacionais com afastamento maior do que 15 dias. Usar este fator para considerar que a geração de benefícios seguirá a mesma proporção no futuro.</t>
+  </si>
+  <si>
+    <t>Inserir as variáveis como parâmetros: 
+FatorB91
+FatorB92
+FatorB93
+FatorB94</t>
   </si>
 </sst>
 </file>
@@ -274,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -285,10 +292,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,24 +983,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>22</v>
+      <c r="F17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Substituindo dados de Teste
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>Caso</t>
   </si>
@@ -35,66 +35,27 @@
     <t>Módulo</t>
   </si>
   <si>
-    <t>Qualidade</t>
-  </si>
-  <si>
     <t>Questão</t>
   </si>
   <si>
-    <t>Ganho de Qualidade é difícil de mensurar utilizando diretamente a produção projetada.</t>
-  </si>
-  <si>
     <t>Endereçamento</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Reclamatórias Trabalhistas</t>
-  </si>
-  <si>
-    <t>O número de funcionários desligados acumulado é de difícil obtenção e vinculação ao número de reclamatórias.</t>
-  </si>
-  <si>
-    <t>Ganho de qualidade será estimado diretamente.</t>
-  </si>
-  <si>
-    <t>Produtividade</t>
-  </si>
-  <si>
-    <t>Ganho de Produtividade estimado por meio de um saving unitário é de difícil estimação, considerando que a empresa tem um amplo mix.</t>
-  </si>
-  <si>
-    <t>Ganho de Produtividade será estimado diretamente.</t>
-  </si>
-  <si>
     <t>O número de funcionários desligados do ano será usado como mutliplicador da probabilidade de reclamatórias.</t>
   </si>
   <si>
-    <t>FAP</t>
-  </si>
-  <si>
     <t>Erro corrigido.</t>
   </si>
   <si>
-    <t>Despesa do FAP anual possuía um erro no calculo (não apresenta variabilidade).</t>
-  </si>
-  <si>
     <t>Infraestrutura</t>
   </si>
   <si>
-    <t>Seed do modelo é totalmente variável (inclusive variando custos na mesma replicação entre iniciativas).</t>
-  </si>
-  <si>
     <t>Implementar Flag na aba parâmetros para especificar Seed Fixa ou Variável. A Seed somente será variável para parâmetros relacionados à probabilidade de acidentes.</t>
   </si>
   <si>
-    <t>Eventos</t>
-  </si>
-  <si>
-    <t>Distribuição Triangular representa óbitos de modo inadequado.</t>
-  </si>
-  <si>
     <t>Pendente.</t>
   </si>
   <si>
@@ -104,27 +65,15 @@
     <t>Implementar Regressões como etapa de pré-processamento.</t>
   </si>
   <si>
-    <t>Regressão do FAP permite que percentis assumam valores maiores do que 100.</t>
-  </si>
-  <si>
     <t>Implementar "batentes" nas variáveis dos percentis (no mínimo 0 e no máximo 100).</t>
   </si>
   <si>
-    <t>Seguro Patrimonial</t>
-  </si>
-  <si>
     <t>Implementar distribuição "normal truncada".</t>
   </si>
   <si>
-    <t>Eventos e outras variáveis aleatórias podem assumir valores negativos, considerando que a distribuição normal é infinita para os dois lados.</t>
-  </si>
-  <si>
     <t>Implementar função para verificação dos dados de entrada e exibição de um alerta para o usuário. Não somar benefícios entre iniciativas nesse caso.</t>
   </si>
   <si>
-    <t>Uma possível categoria de benefício é a redução do valor de uma seguro patrimonial. Esta categoria não foi mencionada durante os encontros de Pensamento Sistêmico, nem mencionadas na literatura.</t>
-  </si>
-  <si>
     <t>Implementar categoria "Seguro Patrimonial", considerando um valor de benefício informado.</t>
   </si>
   <si>
@@ -144,12 +93,6 @@
   </si>
   <si>
     <t>Melhorar template de dados de entrada separando Dados da Empresa e Planilha do Analista.</t>
-  </si>
-  <si>
-    <t>Índices Máximos para Ganho de Receita por Imagem: Atualmente o índice máximo considerado é o ampliado. No entanto, o índice ampliado é de difícil sensibilidade para o usuário. Além disso, pode ser mais coerente retirar este limite, visto que o ganho será arbitrado.</t>
-  </si>
-  <si>
-    <t>Interdição Operacional</t>
   </si>
   <si>
     <t>As variáveis "dias de interdição" são de difícil obtenção. Além disso, o Lucro Cessante por óbito, outros eventos ou interdição são potencialmente diferentes.</t>
@@ -208,9 +151,6 @@
     <t>GanhoProdutividade deve ser estimado como parâmetro.</t>
   </si>
   <si>
-    <t>Imagem, Índices de Frequência</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Usar padrão da NBR 14280: Taxa de Frequência e Gravidade.</t>
   </si>
@@ -218,9 +158,6 @@
     <t xml:space="preserve">Inserir estas variáveis no template: TempoComputadoMedio (Parâmetro)
 DiasUteis (Dados Projetados)
 </t>
-  </si>
-  <si>
-    <t>O número de benefícios estimados de acordo com os eventos e de acordo com a tabela dos eventos não é aderente aos dados observados no FAP.</t>
   </si>
   <si>
     <t>Calcular um Fator para cada benefício (B91, B92, B94) e os eventos típicos e doenças ocupacionais com afastamento maior do que 15 dias. Usar este fator para considerar que a geração de benefícios seguirá a mesma proporção no futuro.</t>
@@ -231,6 +168,75 @@
 FatorB92
 FatorB93
 FatorB94</t>
+  </si>
+  <si>
+    <t>Texto - Versão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualidade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produtividade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reclamatórias Trabalhistas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infraestrutura. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguro Patrimonial. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem, Índices de Frequência. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interdição Operacional. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O número de benefícios estimados de acordo com os eventos e de acordo com a tabela dos eventos não é aderente aos dados observados no FAP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Índices Máximos para Ganho de Receita por Imagem: Atualmente o índice máximo considerado é o ampliado. No entanto, o índice ampliado é de difícil sensibilidade para o usuário. Além disso, pode ser mais coerente retirar este limite, visto que o ganho será arbitrado. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uma possível categoria de benefício é a redução do valor de uma seguro patrimonial. Esta categoria não foi mencionada durante os encontros de Pensamento Sistêmico, nem mencionadas na literatura. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventos e outras variáveis aleatórias podem assumir valores negativos, considerando que a distribuição normal é infinita para os dois lados. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regressão do FAP permite que percentis assumam valores maiores do que 100. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribuição Triangular representa óbitos de modo inadequado. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed do modelo é totalmente variável (inclusive variando custos na mesma replicação entre iniciativas). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Despesa do FAP anual possuía um erro no calculo (não apresenta variabilidade). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O número de funcionários desligados acumulado é de difícil obtenção e vinculação ao número de reclamatórias. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ganho de Produtividade estimado por meio de um saving unitário é de difícil estimação, considerando que a empresa tem um amplo mix. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ganho de Qualidade é difícil de mensurar utilizando diretamente a produção projetada. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ganho de qualidade será estimado diretamente. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ganho de Produtividade será estimado diretamente. </t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -292,6 +298,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -608,11 +617,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <dimension ref="A1:G17"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,12 +634,13 @@
     <col min="5" max="5" width="36.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -638,376 +649,442 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f>_xlfn.CONCAT("* ",$C$1,": ",C2,$D$1,": ",D2,$E$1,": ",E2,$G$1,": ",G2)</f>
+        <v>* Módulo: Qualidade. Questão: Ganho de Qualidade é difícil de mensurar utilizando diretamente a produção projetada. Endereçamento: Ganho de qualidade será estimado diretamente. Mudança Necessária no Template de Dados: GanhoQualidade deve ser estimados como parâmetros. Outras variáveis relacionadas podem ser eliminadas (margem, produção projetada, variação em vendas).</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f t="shared" ref="H3:H7" si="0">_xlfn.CONCAT("* ",$C$1,": ",C3,$D$1,": ",D3,$E$1,": ",E3,$G$1,": ",G3)</f>
+        <v>* Módulo: Produtividade. Questão: Ganho de Produtividade estimado por meio de um saving unitário é de difícil estimação, considerando que a empresa tem um amplo mix. Endereçamento: Ganho de Produtividade será estimado diretamente. Mudança Necessária no Template de Dados: GanhoProdutividade deve ser estimado como parâmetro.</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>* Módulo: Reclamatórias Trabalhistas. Questão: O número de funcionários desligados acumulado é de difícil obtenção e vinculação ao número de reclamatórias. Endereçamento: O número de funcionários desligados do ano será usado como mutliplicador da probabilidade de reclamatórias.Mudança Necessária no Template de Dados: Funcionários Desligados Iniciais não precisam ser coletados.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>* Módulo: FAP. Questão: Despesa do FAP anual possuía um erro no calculo (não apresenta variabilidade). Endereçamento: Erro corrigido.Mudança Necessária no Template de Dados: Nenhuma.</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>* Módulo: Infraestrutura. Questão: Seed do modelo é totalmente variável (inclusive variando custos na mesma replicação entre iniciativas). Endereçamento: Implementar Flag na aba parâmetros para especificar Seed Fixa ou Variável. A Seed somente será variável para parâmetros relacionados à probabilidade de acidentes.Mudança Necessária no Template de Dados: Coluna SEEDFixa deve estar presente na aba de parâmetros. Lista dos parâmetros sem SeedFIXA deve ser inserida em uma aba.</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>* Módulo: Eventos. Questão: Distribuição Triangular representa óbitos de modo inadequado. Endereçamento: Implementar distribuição de Poisson para os eventos raros (onde não há histórico).Mudança Necessária no Template de Dados: A variável "FuncionariosBase" deve ser incluida na aba "Configs", e é usada pelo modelo para normalizar a taxa de acidentes. O valor deve corresponder à média do número de funcionários projetados.</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" ref="H9:H10" si="1">_xlfn.CONCAT("* ",$C$1,": ",C9,$D$1,": ",D9,$E$1,": ",E9,$G$1,": ",G9)</f>
+        <v>* Módulo: FAP. Questão: Regressão do FAP permite que percentis assumam valores maiores do que 100. Endereçamento: Implementar "batentes" nas variáveis dos percentis (no mínimo 0 e no máximo 100).Mudança Necessária no Template de Dados: Nenhuma.</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>* Módulo: Eventos. Questão: Eventos e outras variáveis aleatórias podem assumir valores negativos, considerando que a distribuição normal é infinita para os dois lados. Endereçamento: Implementar distribuição "normal truncada".Mudança Necessária no Template de Dados: Aba de Parâmetros deve usar a distribuição "normaltruncada", e usar os parâmetros 3 e 4 como mínimo e máximo.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="str">
+        <f>_xlfn.CONCAT("* ",$C$1,": ",C12,$D$1,": ",D12,$E$1,": ",E12,$G$1,": ",G12)</f>
+        <v>* Módulo: Seguro Patrimonial. Questão: Uma possível categoria de benefício é a redução do valor de uma seguro patrimonial. Esta categoria não foi mencionada durante os encontros de Pensamento Sistêmico, nem mencionadas na literatura. Endereçamento: Implementar categoria "Seguro Patrimonial", considerando um valor de benefício informado.Mudança Necessária no Template de Dados: Informar variável DespesasSeguroPatrimonial como parâmetro.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>39</v>
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H14" s="3" t="str">
+        <f t="shared" ref="H14:H15" si="2">_xlfn.CONCAT("* ",$C$1,": ",C14,$D$1,": ",D14,$E$1,": ",E14,$G$1,": ",G14)</f>
+        <v xml:space="preserve">* Módulo: Imagem, Índices de Frequência. Questão: Índices Máximos para Ganho de Receita por Imagem: Atualmente o índice máximo considerado é o ampliado. No entanto, o índice ampliado é de difícil sensibilidade para o usuário. Além disso, pode ser mais coerente retirar este limite, visto que o ganho será arbitrado. Endereçamento: 
+Usar padrão da NBR 14280: Taxa de Frequência e Gravidade.Mudança Necessária no Template de Dados: Inserir estas variáveis no template: TempoComputadoMedio (Parâmetro)
+DiasUteis (Dados Projetados)
+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>* Módulo: Interdição Operacional. Questão: As variáveis "dias de interdição" são de difícil obtenção. Além disso, o Lucro Cessante por óbito, outros eventos ou interdição são potencialmente diferentes.Endereçamento: Separar o Lucro Cessante para cada tipo de interdição e estimar diretamente o lucro cessante total por evento.Mudança Necessária no Template de Dados: Estas Variáveis devem ser estimadas como parâmetros: LucroCessanteAcidenteObito
+LucroCessanteAcidenteOutros
+LucroCessanteInterdicaoFiscalizacao</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>64</v>
+        <v>43</v>
+      </c>
+      <c r="H17" s="3" t="str">
+        <f>_xlfn.CONCAT("* ",$C$1,": ",C17,$D$1,": ",D17,$E$1,": ",E17,$G$1,": ",G17)</f>
+        <v>* Módulo: Eventos. Questão: O número de benefícios estimados de acordo com os eventos e de acordo com a tabela dos eventos não é aderente aos dados observados no FAP. Endereçamento: Calcular um Fator para cada benefício (B91, B92, B94) e os eventos típicos e doenças ocupacionais com afastamento maior do que 15 dias. Usar este fator para considerar que a geração de benefícios seguirá a mesma proporção no futuro.Mudança Necessária no Template de Dados: Inserir as variáveis como parâmetros: 
+FatorB91
+FatorB92
+FatorB93
+FatorB94</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F15" xr:uid="{6E59EE85-8273-468A-A589-1946F5BAD21C}"/>
+  <autoFilter ref="A1:F17" xr:uid="{6E59EE85-8273-468A-A589-1946F5BAD21C}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Mudança Implementada, Testar"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Alterações na Versão da Calculadora
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -298,9 +298,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,9 +617,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,13 +668,13 @@
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -698,13 +695,13 @@
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -725,13 +722,13 @@
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -752,10 +749,10 @@
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -779,10 +776,10 @@
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -806,10 +803,10 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -853,10 +850,10 @@
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -880,10 +877,10 @@
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -927,10 +924,10 @@
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -974,10 +971,10 @@
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>55</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1004,10 +1001,10 @@
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1053,10 +1050,10 @@
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="4" t="s">

</xml_diff>

<commit_message>
Registrando novas alterações (ainda incompleto)
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$K$22</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
   <si>
     <t>Caso</t>
   </si>
@@ -170,9 +170,6 @@
 FatorB94</t>
   </si>
   <si>
-    <t>Texto - Versão</t>
-  </si>
-  <si>
     <t xml:space="preserve">Qualidade. </t>
   </si>
   <si>
@@ -237,6 +234,85 @@
   </si>
   <si>
     <t xml:space="preserve">Ganho de Produtividade será estimado diretamente. </t>
+  </si>
+  <si>
+    <t>Multas</t>
+  </si>
+  <si>
+    <t>Taxas de Gravidade e Regressões</t>
+  </si>
+  <si>
+    <t>Validação de Dados</t>
+  </si>
+  <si>
+    <t>Implementar rotinas de verificação dos dados de entrada.</t>
+  </si>
+  <si>
+    <t>Nos casos apresentados o número de multas históricos foi nulo, dificultando a realização de regressão relacionada ao evento.</t>
+  </si>
+  <si>
+    <t>Implementar nova fórmula de calculo, visto que em diversos casos não será possível realizar uma regressão do número de multas com os eventos.
+Utilizar o mesmo formato de calculo dos Eventos de Interdição.</t>
+  </si>
+  <si>
+    <t>Absenteísmo</t>
+  </si>
+  <si>
+    <t>O custo em absenteísmo não diferencia dias perdidos por afastamento justificado (com atestado), das faltas.</t>
+  </si>
+  <si>
+    <t>A despesa com afastamento justificado deveria ter peso dobrado, visto que a empresa remunera o funcionário pela falta.</t>
+  </si>
+  <si>
+    <t>Modelo Matemático Foi Ajustado?</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Resp.</t>
+  </si>
+  <si>
+    <t>PNL</t>
+  </si>
+  <si>
+    <t>Macro-Módulo</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>LFR</t>
+  </si>
+  <si>
+    <t>Processamento</t>
+  </si>
+  <si>
+    <t>Plano de Saúde</t>
+  </si>
+  <si>
+    <t>As despesas com plano de saúde apresentam comportamento anormal (variam com sinais negativos e positivos anualmente).</t>
+  </si>
+  <si>
+    <t>Há um erro no calculo das despesas com o Plano de Saúde. Corrigir</t>
+  </si>
+  <si>
+    <t>Não é necessário</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Mudança</t>
+  </si>
+  <si>
+    <t>Alterar a forma de calculo E a regra de precedência dos calculos para considerar a nova Taxa de Gravidade e Frequência incorporada ao modelo.</t>
+  </si>
+  <si>
+    <t>As regressões inseridas no modelo utilizam o Índice de Gravidade e Frequência Ampliados, para os quais o usuário do modelo não será sensível.</t>
+  </si>
+  <si>
+    <t>Sem uma rotina de verificação, o modelo pode rodar sem verificar erros "óbvios" (Ex.: Número de funcionários igual a zero).</t>
   </si>
 </sst>
 </file>
@@ -267,12 +343,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -287,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -298,6 +380,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,28 +700,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="63.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="16.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="63.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46" style="4" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -643,187 +730,244 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="3" t="str">
-        <f>_xlfn.CONCAT("* ",$C$1,": ",C2,$D$1,": ",D2,$E$1,": ",E2,$G$1,": ",G2)</f>
-        <v>* Módulo: Qualidade. Questão: Ganho de Qualidade é difícil de mensurar utilizando diretamente a produção projetada. Endereçamento: Ganho de qualidade será estimado diretamente. Mudança Necessária no Template de Dados: GanhoQualidade deve ser estimados como parâmetros. Outras variáveis relacionadas podem ser eliminadas (margem, produção projetada, variação em vendas).</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="J3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="str">
-        <f t="shared" ref="H3:H7" si="0">_xlfn.CONCAT("* ",$C$1,": ",C3,$D$1,": ",D3,$E$1,": ",E3,$G$1,": ",G3)</f>
-        <v>* Módulo: Produtividade. Questão: Ganho de Produtividade estimado por meio de um saving unitário é de difícil estimação, considerando que a empresa tem um amplo mix. Endereçamento: Ganho de Produtividade será estimado diretamente. Mudança Necessária no Template de Dados: GanhoProdutividade deve ser estimado como parâmetro.</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="K3" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>47</v>
+      <c r="C4" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>* Módulo: Reclamatórias Trabalhistas. Questão: O número de funcionários desligados acumulado é de difícil obtenção e vinculação ao número de reclamatórias. Endereçamento: O número de funcionários desligados do ano será usado como mutliplicador da probabilidade de reclamatórias.Mudança Necessária no Template de Dados: Funcionários Desligados Iniciais não precisam ser coletados.</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="K4" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>* Módulo: FAP. Questão: Despesa do FAP anual possuía um erro no calculo (não apresenta variabilidade). Endereçamento: Erro corrigido.Mudança Necessária no Template de Dados: Nenhuma.</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>* Módulo: Infraestrutura. Questão: Seed do modelo é totalmente variável (inclusive variando custos na mesma replicação entre iniciativas). Endereçamento: Implementar Flag na aba parâmetros para especificar Seed Fixa ou Variável. A Seed somente será variável para parâmetros relacionados à probabilidade de acidentes.Mudança Necessária no Template de Dados: Coluna SEEDFixa deve estar presente na aba de parâmetros. Lista dos parâmetros sem SeedFIXA deve ser inserida em uma aba.</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="J7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>* Módulo: Eventos. Questão: Distribuição Triangular representa óbitos de modo inadequado. Endereçamento: Implementar distribuição de Poisson para os eventos raros (onde não há histórico).Mudança Necessária no Template de Dados: A variável "FuncionariosBase" deve ser incluida na aba "Configs", e é usada pelo modelo para normalizar a taxa de acidentes. O valor deve corresponder à média do número de funcionários projetados.</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -831,120 +975,162 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="K8" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
+      <c r="C9" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="3" t="str">
-        <f t="shared" ref="H9:H10" si="1">_xlfn.CONCAT("* ",$C$1,": ",C9,$D$1,": ",D9,$E$1,": ",E9,$G$1,": ",G9)</f>
-        <v>* Módulo: FAP. Questão: Regressão do FAP permite que percentis assumam valores maiores do que 100. Endereçamento: Implementar "batentes" nas variáveis dos percentis (no mínimo 0 e no máximo 100).Mudança Necessária no Template de Dados: Nenhuma.</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="K9" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="I10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="J10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>* Módulo: Eventos. Questão: Eventos e outras variáveis aleatórias podem assumir valores negativos, considerando que a distribuição normal é infinita para os dois lados. Endereçamento: Implementar distribuição "normal truncada".Mudança Necessária no Template de Dados: Aba de Parâmetros deve usar a distribuição "normaltruncada", e usar os parâmetros 3 e 4 como mínimo e máximo.</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="K11" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="I12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="J12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="3" t="str">
-        <f>_xlfn.CONCAT("* ",$C$1,": ",C12,$D$1,": ",D12,$E$1,": ",E12,$G$1,": ",G12)</f>
-        <v>* Módulo: Seguro Patrimonial. Questão: Uma possível categoria de benefício é a redução do valor de uma seguro patrimonial. Esta categoria não foi mencionada durante os encontros de Pensamento Sistêmico, nem mencionadas na literatura. Endereçamento: Implementar categoria "Seguro Patrimonial", considerando um valor de benefício informado.Mudança Necessária no Template de Dados: Informar variável DespesasSeguroPatrimonial como parâmetro.</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -952,78 +1138,101 @@
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="K13" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>52</v>
+      <c r="C14" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="3" t="str">
-        <f t="shared" ref="H14:H15" si="2">_xlfn.CONCAT("* ",$C$1,": ",C14,$D$1,": ",D14,$E$1,": ",E14,$G$1,": ",G14)</f>
-        <v xml:space="preserve">* Módulo: Imagem, Índices de Frequência. Questão: Índices Máximos para Ganho de Receita por Imagem: Atualmente o índice máximo considerado é o ampliado. No entanto, o índice ampliado é de difícil sensibilidade para o usuário. Além disso, pode ser mais coerente retirar este limite, visto que o ganho será arbitrado. Endereçamento: 
-Usar padrão da NBR 14280: Taxa de Frequência e Gravidade.Mudança Necessária no Template de Dados: Inserir estas variáveis no template: TempoComputadoMedio (Parâmetro)
-DiasUteis (Dados Projetados)
-</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="K14" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>53</v>
+      <c r="C15" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>* Módulo: Interdição Operacional. Questão: As variáveis "dias de interdição" são de difícil obtenção. Além disso, o Lucro Cessante por óbito, outros eventos ou interdição são potencialmente diferentes.Endereçamento: Separar o Lucro Cessante para cada tipo de interdição e estimar diretamente o lucro cessante total por evento.Mudança Necessária no Template de Dados: Estas Variáveis devem ser estimadas como parâmetros: LucroCessanteAcidenteObito
-LucroCessanteAcidenteOutros
-LucroCessanteInterdicaoFiscalizacao</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1031,57 +1240,224 @@
         <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="K16" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>50</v>
+      <c r="C17" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="J17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="3" t="str">
-        <f>_xlfn.CONCAT("* ",$C$1,": ",C17,$D$1,": ",D17,$E$1,": ",E17,$G$1,": ",G17)</f>
-        <v>* Módulo: Eventos. Questão: O número de benefícios estimados de acordo com os eventos e de acordo com a tabela dos eventos não é aderente aos dados observados no FAP. Endereçamento: Calcular um Fator para cada benefício (B91, B92, B94) e os eventos típicos e doenças ocupacionais com afastamento maior do que 15 dias. Usar este fator para considerar que a geração de benefícios seguirá a mesma proporção no futuro.Mudança Necessária no Template de Dados: Inserir as variáveis como parâmetros: 
-FatorB91
-FatorB92
-FatorB93
-FatorB94</v>
-      </c>
+      <c r="K17" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F17" xr:uid="{6E59EE85-8273-468A-A589-1946F5BAD21C}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Mudança Implementada, Testar"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K22" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Inserção de outros itens pendentes
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="110">
   <si>
     <t>Caso</t>
   </si>
@@ -313,6 +313,60 @@
   </si>
   <si>
     <t>Sem uma rotina de verificação, o modelo pode rodar sem verificar erros "óbvios" (Ex.: Número de funcionários igual a zero).</t>
+  </si>
+  <si>
+    <t>Ações Regressivas INSS</t>
+  </si>
+  <si>
+    <t>O calculo das ações regressivas realiza uma ponderação do custo médio dos benefícios, o que pode trazer distorções para o calculo da despesa com ações regressivas.</t>
+  </si>
+  <si>
+    <t>Individualizar o calculo das ações regressivas por benefício.</t>
+  </si>
+  <si>
+    <t>Erro</t>
+  </si>
+  <si>
+    <t>Calculo Flexível das Categorias (calculo simplificado).</t>
+  </si>
+  <si>
+    <t>Validação de Regressões (Beta 1 &lt; 0 significa na maioria dos casos que os dados históricos não suportam relação positiva entre acidentes e despesas).</t>
+  </si>
+  <si>
+    <t>Escopo</t>
+  </si>
+  <si>
+    <t>Delay em Parâmetros.</t>
+  </si>
+  <si>
+    <t>Previsto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soma dos Benefícios e Custos entre Iniciativas</t>
+  </si>
+  <si>
+    <t>Relatório em PDF e Gráficos de Outputs da Calculadora;</t>
+  </si>
+  <si>
+    <t>Soma dos benefícios condicional (opcional);</t>
+  </si>
+  <si>
+    <t>Outputs dos parâmetros no relatório</t>
+  </si>
+  <si>
+    <t>DBG</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Versão Final do App Shiny</t>
+  </si>
+  <si>
+    <t>DBG/LFR</t>
+  </si>
+  <si>
+    <t>Planilha do Analista e Empresa de acordo com processo simplificado e condicional.</t>
   </si>
 </sst>
 </file>
@@ -343,18 +397,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -379,11 +427,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -700,11 +748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,704 +805,1010 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="K2" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="K3" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="K4" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="K5" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="E6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="K6" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="E7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="K7" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="F8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="K9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="E10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="K10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="E12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="K12" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="F13" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="B14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="E14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="K14" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="E15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="K15" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="F16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="J16" s="6"/>
+      <c r="K16" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="K17" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="B19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="J19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="B20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="E20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="J20" s="6"/>
+      <c r="K20" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="B21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="4" t="s">
+      <c r="E21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="J21" s="6"/>
+      <c r="K21" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="B22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="E22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
+    <row r="23" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K22" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}"/>

</xml_diff>

<commit_message>
Adicionando alterações aos Casos.
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="110">
   <si>
     <t>Caso</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Infraestrutura</t>
-  </si>
-  <si>
-    <t>Implementar Flag na aba parâmetros para especificar Seed Fixa ou Variável. A Seed somente será variável para parâmetros relacionados à probabilidade de acidentes.</t>
   </si>
   <si>
     <t>Pendente.</t>
@@ -367,6 +364,9 @@
   </si>
   <si>
     <t>Planilha do Analista e Empresa de acordo com processo simplificado e condicional.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar Flag na aba parâmetros para especificar Seed Fixa ou Variável. </t>
   </si>
 </sst>
 </file>
@@ -748,12 +748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,22 +772,22 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -800,331 +799,331 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="I2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="K7" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="I8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
@@ -1132,226 +1131,226 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="F13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="I13" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="K14" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="I15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="I16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="K17" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1359,32 +1358,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="I18" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1392,32 +1391,32 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="I19" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1425,100 +1424,102 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="I20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="I21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="K21" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1526,32 +1527,32 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="I23" s="5" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1559,26 +1560,26 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1588,26 +1589,26 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -1617,26 +1618,26 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -1646,189 +1647,177 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="F32" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K32" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="PNL"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Backlog Pós-Piloto."/>
-        <filter val="Pendente."/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K32" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando Item do Fator de Ajuste - Taxas de Frequência e Gravidade
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="115">
   <si>
     <t>Caso</t>
   </si>
@@ -367,6 +367,21 @@
   </si>
   <si>
     <t xml:space="preserve">Implementar Flag na aba parâmetros para especificar Seed Fixa ou Variável. </t>
+  </si>
+  <si>
+    <t>Homem Horas de Exposição ao Risco pode não corresponder com o número total de homem horas trabalhada.</t>
+  </si>
+  <si>
+    <t>Implementar "Fator de Ajuste" para o calculo das Taxas de Frequência e Gravidade.</t>
+  </si>
+  <si>
+    <t>Pendente (Testar)</t>
+  </si>
+  <si>
+    <t>Pirelli</t>
+  </si>
+  <si>
+    <t>Criar Variável Homem Hora Exposição ao Risco.</t>
   </si>
 </sst>
 </file>
@@ -748,11 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,6 +1831,41 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K32" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualizando Lista de Alterações
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$K$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$K$33</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -339,9 +339,6 @@
     <t>Previsto</t>
   </si>
   <si>
-    <t xml:space="preserve"> Soma dos Benefícios e Custos entre Iniciativas</t>
-  </si>
-  <si>
     <t>Relatório em PDF e Gráficos de Outputs da Calculadora;</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>Criar Variável Homem Hora Exposição ao Risco.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soma dos Benefícios e Custos entre Iniciativas - Isso não foi realizado nos pilotos.</t>
   </si>
 </sst>
 </file>
@@ -763,11 +763,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +821,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -855,7 +856,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -890,7 +891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -925,7 +926,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -960,7 +961,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -983,7 +984,7 @@
         <v>58</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>36</v>
@@ -995,7 +996,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1098,7 +1099,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1467,7 +1468,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1657,7 +1658,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>99</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
@@ -1686,7 +1687,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1694,19 +1695,19 @@
         <v>97</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
@@ -1715,7 +1716,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1723,19 +1724,19 @@
         <v>97</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
@@ -1744,7 +1745,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1752,19 +1753,19 @@
         <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
@@ -1773,7 +1774,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1781,19 +1782,19 @@
         <v>97</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
@@ -1802,7 +1803,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1822,7 +1823,7 @@
         <v>99</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
@@ -1836,7 +1837,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>81</v>
@@ -1851,23 +1852,35 @@
         <v>87</v>
       </c>
       <c r="G33" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="J33" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K32" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}"/>
+  <autoFilter ref="A1:K33" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="PNL"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Pendente (Testar)"/>
+        <filter val="Pendente."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustando verificações no modelo
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -768,7 +768,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
atualizando planilha de alterações e Dados
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$K$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$K$31</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="115">
   <si>
     <t>Caso</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>Coluna SEEDFixa deve estar presente na aba de parâmetros. Lista dos parâmetros sem SeedFIXA deve ser inserida em uma aba.</t>
-  </si>
-  <si>
-    <t>Backlog Pós-Piloto.</t>
   </si>
   <si>
     <t>Aba de Parâmetros deve usar a distribuição "normaltruncada", e usar os parâmetros 3 e 4 como mínimo e máximo.</t>
@@ -327,9 +324,6 @@
     <t>Calculo Flexível das Categorias (calculo simplificado).</t>
   </si>
   <si>
-    <t>Validação de Regressões (Beta 1 &lt; 0 significa na maioria dos casos que os dados históricos não suportam relação positiva entre acidentes e despesas).</t>
-  </si>
-  <si>
     <t>Escopo</t>
   </si>
   <si>
@@ -345,21 +339,9 @@
     <t>Soma dos benefícios condicional (opcional);</t>
   </si>
   <si>
-    <t>Outputs dos parâmetros no relatório</t>
-  </si>
-  <si>
-    <t>DBG</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
-    <t>Versão Final do App Shiny</t>
-  </si>
-  <si>
-    <t>DBG/LFR</t>
-  </si>
-  <si>
     <t>Planilha do Analista e Empresa de acordo com processo simplificado e condicional.</t>
   </si>
   <si>
@@ -372,9 +354,6 @@
     <t>Implementar "Fator de Ajuste" para o calculo das Taxas de Frequência e Gravidade.</t>
   </si>
   <si>
-    <t>Pendente (Testar)</t>
-  </si>
-  <si>
     <t>Pirelli</t>
   </si>
   <si>
@@ -382,6 +361,28 @@
   </si>
   <si>
     <t xml:space="preserve"> Soma dos Benefícios e Custos entre Iniciativas - Isso não foi realizado nos pilotos.</t>
+  </si>
+  <si>
+    <t>Validação de Regressões (Beta 1 &lt; 0 significa na maioria dos casos que os dados históricos não suportam relação positiva entre acidentes e despesas).
+Inserir batentes em regressões.</t>
+  </si>
+  <si>
+    <t>Inserir anos de delay em parâmetros.</t>
+  </si>
+  <si>
+    <t>Implementar batentes</t>
+  </si>
+  <si>
+    <t>Testar erros de inserção de dados.</t>
+  </si>
+  <si>
+    <t>Implementar calculo flexível também do FAP (atualmente está como obrigatório).</t>
+  </si>
+  <si>
+    <t>Verificar erros quando os dados não são numéricos, ou os parâmetros são incoerentes.</t>
+  </si>
+  <si>
+    <t>Verificar nova implementação.</t>
   </si>
 </sst>
 </file>
@@ -432,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,6 +448,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -764,11 +768,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,16 +798,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -818,10 +822,10 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -829,34 +833,34 @@
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="I2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -864,34 +868,34 @@
         <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -899,34 +903,34 @@
         <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -934,34 +938,34 @@
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -969,34 +973,34 @@
         <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1004,31 +1008,31 @@
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="K7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1039,16 +1043,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>9</v>
@@ -1056,15 +1060,15 @@
       <c r="H8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>28</v>
+      <c r="I8" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1072,34 +1076,34 @@
         <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1107,47 +1111,51 @@
         <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>80</v>
+      </c>
       <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="F11" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>17</v>
@@ -1155,15 +1163,15 @@
       <c r="H11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>28</v>
+      <c r="I11" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1171,31 +1179,31 @@
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -1206,16 +1214,16 @@
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>19</v>
@@ -1228,10 +1236,10 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1239,34 +1247,34 @@
         <v>15</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="K14" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1274,16 +1282,16 @@
         <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>21</v>
@@ -1292,13 +1300,13 @@
         <v>22</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>24</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1306,35 +1314,35 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1342,31 +1350,31 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="K17" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1374,32 +1382,32 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>8</v>
+      <c r="I18" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1410,32 +1418,32 @@
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>8</v>
+      <c r="I19" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1443,67 +1451,67 @@
         <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>8</v>
+      <c r="I20" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="I21" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>26</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1511,34 +1519,34 @@
         <v>15</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1546,114 +1554,116 @@
         <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="I23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="5" t="s">
-        <v>8</v>
+      <c r="I24" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="H25" s="5"/>
-      <c r="I25" s="5" t="s">
-        <v>8</v>
+      <c r="I25" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5" t="s">
-        <v>8</v>
+        <v>96</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -1663,22 +1673,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
@@ -1687,27 +1697,27 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="G28" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
@@ -1716,27 +1726,27 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
@@ -1745,27 +1755,27 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="G30" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
@@ -1774,110 +1784,46 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="B31" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="I31" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>32</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>75</v>
+      <c r="K31" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K33" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}">
+  <autoFilter ref="A1:K31" xr:uid="{B8F59C8B-6412-4867-A0B5-4900F1B49B5D}">
     <filterColumn colId="4">
       <filters>
         <filter val="PNL"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Pendente (Testar)"/>
-        <filter val="Pendente."/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Iniciando verificação de estimativas das iniciativas, e soma de custos e benefícios.
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="114">
   <si>
     <t>Caso</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>Verificar erros quando os dados não são numéricos, ou os parâmetros são incoerentes.</t>
-  </si>
-  <si>
-    <t>Verificar nova implementação.</t>
   </si>
 </sst>
 </file>
@@ -771,8 +768,8 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +822,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -860,7 +857,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -895,7 +892,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -930,7 +927,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -965,7 +962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1000,7 +997,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1068,7 +1065,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1239,7 +1236,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1274,7 +1271,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1403,14 +1400,14 @@
         <v>69</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1511,7 +1508,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1546,7 +1543,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1784,7 +1781,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1826,6 +1823,16 @@
         <filter val="PNL"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Implementar batentes"/>
+        <filter val="Implementar calculo flexível também do FAP (atualmente está como obrigatório)."/>
+        <filter val="Pendente."/>
+        <filter val="Testar erros de inserção de dados."/>
+        <filter val="Verificar erros quando os dados não são numéricos, ou os parâmetros são incoerentes."/>
+        <filter val="Verificar nova implementação."/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revisando batentes e constantes
</commit_message>
<xml_diff>
--- a/tests/testthat/Alteracoes_Casos.xlsx
+++ b/tests/testthat/Alteracoes_Casos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="116">
   <si>
     <t>Caso</t>
   </si>
@@ -164,33 +164,6 @@
 FatorB94</t>
   </si>
   <si>
-    <t xml:space="preserve">Qualidade. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produtividade. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reclamatórias Trabalhistas. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAP. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infraestrutura. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eventos. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seguro Patrimonial. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imagem, Índices de Frequência. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interdição Operacional. </t>
-  </si>
-  <si>
     <t xml:space="preserve">O número de benefícios estimados de acordo com os eventos e de acordo com a tabela dos eventos não é aderente aos dados observados no FAP. </t>
   </si>
   <si>
@@ -363,23 +336,55 @@
     <t xml:space="preserve"> Soma dos Benefícios e Custos entre Iniciativas - Isso não foi realizado nos pilotos.</t>
   </si>
   <si>
-    <t>Validação de Regressões (Beta 1 &lt; 0 significa na maioria dos casos que os dados históricos não suportam relação positiva entre acidentes e despesas).
-Inserir batentes em regressões.</t>
-  </si>
-  <si>
     <t>Inserir anos de delay em parâmetros.</t>
   </si>
   <si>
-    <t>Implementar batentes</t>
-  </si>
-  <si>
-    <t>Testar erros de inserção de dados.</t>
-  </si>
-  <si>
-    <t>Implementar calculo flexível também do FAP (atualmente está como obrigatório).</t>
-  </si>
-  <si>
-    <t>Verificar erros quando os dados não são numéricos, ou os parâmetros são incoerentes.</t>
+    <t>Implementar versão básica, simplificada e customizada.</t>
+  </si>
+  <si>
+    <t>Validação de Regressões (Beta 1 &lt; 0 significa na maioria dos casos que os dados históricos não suportam relação positiva entre acidentes e despesas). Inserir batentes em regressões.</t>
+  </si>
+  <si>
+    <t>Implementar limites superiores e inferiores para as regressões, e verificação relacionada à coerência do Beta 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qualidade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produtividade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reclamatórias Trabalhistas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infraestrutura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguro Patrimonial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagem, Índices de Frequência </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interdição Operacional </t>
+  </si>
+  <si>
+    <t>Implementar mecanismos de logs para a calculadora. Os logs devem ser exportados como um resultado da simulação, assim como os próprios resultados da simulação.</t>
+  </si>
+  <si>
+    <t>Em alguns casos é importante que o usuário do modelo receba informação sobre a utilização dos batentes utilizados nas regressões, para posterior verificação do calculo do CBR.</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -430,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -450,6 +455,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,11 +774,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313E83F6-F2EB-4DBF-92CC-1536BAC0A730}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +787,7 @@
     <col min="2" max="2" width="9.140625" style="7"/>
     <col min="3" max="3" width="16.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="7" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="63.5703125" style="7" customWidth="1"/>
     <col min="8" max="8" width="36.42578125" style="7" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -795,16 +804,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -819,10 +828,10 @@
         <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -830,22 +839,22 @@
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>35</v>
@@ -854,10 +863,10 @@
         <v>36</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -865,22 +874,22 @@
         <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>35</v>
@@ -889,10 +898,10 @@
         <v>37</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -900,19 +909,19 @@
         <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>5</v>
@@ -924,10 +933,10 @@
         <v>25</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -935,19 +944,19 @@
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>6</v>
@@ -959,10 +968,10 @@
         <v>26</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -970,22 +979,22 @@
         <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>35</v>
@@ -994,10 +1003,10 @@
         <v>27</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1005,19 +1014,19 @@
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>30</v>
@@ -1029,7 +1038,7 @@
         <v>31</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1040,16 +1049,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>9</v>
@@ -1062,10 +1071,10 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1073,19 +1082,19 @@
         <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>11</v>
@@ -1097,10 +1106,10 @@
         <v>26</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1108,19 +1117,19 @@
         <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>12</v>
@@ -1132,7 +1141,7 @@
         <v>28</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1143,16 +1152,16 @@
         <v>15</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>17</v>
@@ -1161,14 +1170,14 @@
         <v>13</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1176,19 +1185,19 @@
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>14</v>
@@ -1200,7 +1209,7 @@
         <v>29</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -1211,16 +1220,16 @@
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>19</v>
@@ -1233,10 +1242,10 @@
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1244,19 +1253,19 @@
         <v>15</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>38</v>
@@ -1268,10 +1277,10 @@
         <v>39</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1279,16 +1288,16 @@
         <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>21</v>
@@ -1303,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1314,16 +1323,16 @@
         <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>33</v>
@@ -1336,10 +1345,10 @@
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1347,19 +1356,19 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>40</v>
@@ -1371,7 +1380,7 @@
         <v>41</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1382,32 +1391,32 @@
         <v>32</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>35</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1415,32 +1424,32 @@
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>35</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1448,32 +1457,32 @@
         <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="H20" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1481,22 +1490,22 @@
         <v>32</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>35</v>
@@ -1505,7 +1514,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1516,22 +1525,22 @@
         <v>15</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>35</v>
@@ -1540,10 +1549,10 @@
         <v>26</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1551,32 +1560,32 @@
         <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1584,23 +1593,25 @@
         <v>32</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="I24" s="8" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1613,141 +1624,143 @@
         <v>32</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H25" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="I25" s="8" t="s">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="H27" s="5"/>
-      <c r="I27" s="5" t="s">
-        <v>8</v>
+      <c r="I27" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="5" t="s">
-        <v>8</v>
+      <c r="I28" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="5" t="s">
-        <v>8</v>
+      <c r="I29" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1757,22 +1770,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
@@ -1781,39 +1794,68 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>35</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1823,14 +1865,9 @@
         <filter val="PNL"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="8">
+    <filterColumn colId="5">
       <filters>
-        <filter val="Implementar batentes"/>
-        <filter val="Implementar calculo flexível também do FAP (atualmente está como obrigatório)."/>
-        <filter val="Pendente."/>
-        <filter val="Testar erros de inserção de dados."/>
-        <filter val="Verificar erros quando os dados não são numéricos, ou os parâmetros são incoerentes."/>
-        <filter val="Verificar nova implementação."/>
+        <filter val="Mudança"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>